<commit_message>
inscription BO queue consumer
</commit_message>
<xml_diff>
--- a/Stubs/queueName.xlsx
+++ b/Stubs/queueName.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calu\Documents\GitHub\MTT\Stubs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Workspace\MiwaMTT\Stubs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Nom queue</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>WAREHOUSE_Receipts</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>CRM_client_&lt;paris&gt;</t>
   </si>
 </sst>
 </file>
@@ -607,21 +613,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="43.6328125" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" customWidth="1"/>
-    <col min="4" max="4" width="32.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -635,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -643,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -651,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -659,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -667,7 +673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -676,7 +682,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -684,15 +690,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -700,7 +709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -708,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -716,7 +725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -724,240 +733,266 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>38</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>47</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>68</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="D38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>69</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>73</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>